<commit_message>
Updated Testing - Modified kh for tension according to German Annex
</commit_message>
<xml_diff>
--- a/StructuraldesignKitTesting/TestData/Test_CrossSections.xlsx
+++ b/StructuraldesignKitTesting/TestData/Test_CrossSections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khing.local\share\users$\gc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc\source\repos\StructuralDesignKit\StructuraldesignKitTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F030C7-446E-4538-B1CD-6AA8177C3936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E993A34-3EAB-4F94-9ED4-C10BA4EF9040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{971BC0E7-8629-419A-B2CB-730A67335DFF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="16">
   <si>
     <t>B</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Ym</t>
   </si>
   <si>
-    <t>Kh</t>
-  </si>
-  <si>
-    <t>Kl_LVL</t>
-  </si>
-  <si>
     <t>Ratio</t>
   </si>
   <si>
@@ -78,6 +72,21 @@
   </si>
   <si>
     <t>Date data</t>
+  </si>
+  <si>
+    <t>RFEM Timber Pro</t>
+  </si>
+  <si>
+    <t>GL28h</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>D30</t>
+  </si>
+  <si>
+    <t>N [kN]</t>
   </si>
 </sst>
 </file>
@@ -121,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -129,6 +138,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -446,32 +456,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D737A44-6696-40E2-A70F-6CB1F0298E3A}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="79.42578125" customWidth="1"/>
+    <col min="1" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="79.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,19 +503,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -514,7 +517,7 @@
         <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>100</v>
@@ -526,16 +529,16 @@
         <v>1.3</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3">
+        <v>44904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100</v>
       </c>
@@ -543,7 +546,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>100</v>
@@ -555,18 +558,314 @@
         <v>1.3</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.03</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3">
+        <v>44904</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>200</v>
+      </c>
+      <c r="B5" s="1">
+        <v>600</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3">
+        <v>44904</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3">
+        <v>44904</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1">
+        <v>160</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3">
+        <v>44904</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>200</v>
+      </c>
+      <c r="B8" s="1">
+        <v>300</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3">
+        <v>44904</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1">
+        <v>200</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45084</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>200</v>
+      </c>
+      <c r="B11" s="1">
+        <v>600</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>80</v>
+      </c>
+      <c r="B12" s="1">
+        <v>120</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1">
+        <v>160</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>200</v>
+      </c>
+      <c r="B14" s="1">
+        <v>300</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3">
+        <v>45084</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -575,12 +874,412 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023A9510-5D9A-4E42-9E75-8B59D1B40438}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1">
+        <v>200</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>200</v>
+      </c>
+      <c r="B5" s="1">
+        <v>600</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3">
+        <v>45086</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45087</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1">
+        <v>160</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3">
+        <v>45088</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>200</v>
+      </c>
+      <c r="B8" s="1">
+        <v>300</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1">
+        <v>200</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45090</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.03</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>200</v>
+      </c>
+      <c r="B11" s="1">
+        <v>600</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3">
+        <v>45092</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>80</v>
+      </c>
+      <c r="B12" s="1">
+        <v>120</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3">
+        <v>45093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1">
+        <v>160</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3">
+        <v>45094</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>200</v>
+      </c>
+      <c r="B14" s="1">
+        <v>300</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3">
+        <v>45095</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update excel file with test data
</commit_message>
<xml_diff>
--- a/StructuraldesignKitTesting/TestData/Test_CrossSections.xlsx
+++ b/StructuraldesignKitTesting/TestData/Test_CrossSections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume Caussarieu\source\repos\StructuralDesignKit_Holz\StructuraldesignKitTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E0EC2E-36EF-4C3A-8D15-D0DE9C2BFFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B05F0D-C5A7-4326-B5B8-F20B77B0E452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11250" activeTab="2" xr2:uid="{971BC0E7-8629-419A-B2CB-730A67335DFF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{971BC0E7-8629-419A-B2CB-730A67335DFF}"/>
   </bookViews>
   <sheets>
     <sheet name="TensionParallelToGrain" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
   <si>
     <t>B</t>
   </si>
@@ -99,13 +121,31 @@
   </si>
   <si>
     <t>Tension parallel to the grain_6.1.2</t>
+  </si>
+  <si>
+    <t>kh</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Stress</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>variation</t>
+  </si>
+  <si>
+    <t>SDK Excel implementation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +161,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,11 +200,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,9 +230,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,20 +553,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D737A44-6696-40E2-A70F-6CB1F0298E3A}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="7" width="8.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="79.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
@@ -512,8 +579,15 @@
       <c r="G1" s="6"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -541,8 +615,23 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>100</v>
       </c>
@@ -570,8 +659,28 @@
       <c r="I3" s="5">
         <v>44904</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="4" t="str" cm="1">
+        <f t="array" ref="K3">_xll.SDK.Utilities.CreateRectangularCrossSection(A3,B3,C3)</f>
+        <v>CS_R_100x200_GL24h</v>
+      </c>
+      <c r="L3" s="8" cm="1">
+        <f t="array" ref="L3">_xll.SDK.CrossSection_StressCompute.NormalForce(D3,K3)</f>
+        <v>5</v>
+      </c>
+      <c r="M3" s="8" cm="1">
+        <f t="array" ref="M3">_xll.SDK.Factors.Kh_Tension(C3,A3,B3)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N3" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L3,C3,E3,F3,M3,1,0),2)</f>
+        <v>0.51</v>
+      </c>
+      <c r="O3" s="9">
+        <f>N3/G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>100</v>
       </c>
@@ -600,8 +709,28 @@
         <v>44904</v>
       </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="4" t="str" cm="1">
+        <f t="array" ref="K4">_xll.SDK.Utilities.CreateRectangularCrossSection(A4,B4,C4)</f>
+        <v>CS_R_100x100_GL24h</v>
+      </c>
+      <c r="L4" s="8" cm="1">
+        <f t="array" ref="L4">_xll.SDK.CrossSection_StressCompute.NormalForce(D4,K4)</f>
+        <v>10</v>
+      </c>
+      <c r="M4" s="8" cm="1">
+        <f t="array" ref="M4">_xll.SDK.Factors.Kh_Tension(C4,A4,B4)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N4" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L4,C4,E4,F4,M4,1,0),2)</f>
+        <v>1.03</v>
+      </c>
+      <c r="O4" s="9">
+        <f t="shared" ref="O4:O14" si="0">N4/G4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>200</v>
       </c>
@@ -630,8 +759,28 @@
         <v>44904</v>
       </c>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="4" t="str" cm="1">
+        <f t="array" ref="K5">_xll.SDK.Utilities.CreateRectangularCrossSection(A5,B5,C5)</f>
+        <v>CS_R_200x600_GL24h</v>
+      </c>
+      <c r="L5" s="8" cm="1">
+        <f t="array" ref="L5">_xll.SDK.CrossSection_StressCompute.NormalForce(D5,K5)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M5" s="8" cm="1">
+        <f t="array" ref="M5">_xll.SDK.Factors.Kh_Tension(C5,A5,B5)</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L5,C5,E5,F5,M5,1,0),2)</f>
+        <v>0.09</v>
+      </c>
+      <c r="O5" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>80</v>
       </c>
@@ -660,8 +809,28 @@
         <v>44904</v>
       </c>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="4" t="str" cm="1">
+        <f t="array" ref="K6">_xll.SDK.Utilities.CreateRectangularCrossSection(A6,B6,C6)</f>
+        <v>CS_R_80x120_GL28h</v>
+      </c>
+      <c r="L6" s="8" cm="1">
+        <f t="array" ref="L6">_xll.SDK.CrossSection_StressCompute.NormalForce(D6,K6)</f>
+        <v>10.416666666666666</v>
+      </c>
+      <c r="M6" s="8" cm="1">
+        <f t="array" ref="M6">_xll.SDK.Factors.Kh_Tension(C6,A6,B6)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N6" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L6,C6,E6,F6,M6,1,0),2)</f>
+        <v>0.69</v>
+      </c>
+      <c r="O6" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>100</v>
       </c>
@@ -690,8 +859,28 @@
         <v>44904</v>
       </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="str" cm="1">
+        <f t="array" ref="K7">_xll.SDK.Utilities.CreateRectangularCrossSection(A7,B7,C7)</f>
+        <v>CS_R_100x160_GL28h</v>
+      </c>
+      <c r="L7" s="8" cm="1">
+        <f t="array" ref="L7">_xll.SDK.CrossSection_StressCompute.NormalForce(D7,K7)</f>
+        <v>6.25</v>
+      </c>
+      <c r="M7" s="8" cm="1">
+        <f t="array" ref="M7">_xll.SDK.Factors.Kh_Tension(C7,A7,B7)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N7" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L7,C7,E7,F7,M7,1,0),2)</f>
+        <v>0.41</v>
+      </c>
+      <c r="O7" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>200</v>
       </c>
@@ -720,8 +909,28 @@
         <v>44904</v>
       </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="4" t="str" cm="1">
+        <f t="array" ref="K8">_xll.SDK.Utilities.CreateRectangularCrossSection(A8,B8,C8)</f>
+        <v>CS_R_200x300_GL28h</v>
+      </c>
+      <c r="L8" s="8" cm="1">
+        <f t="array" ref="L8">_xll.SDK.CrossSection_StressCompute.NormalForce(D8,K8)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M8" s="8" cm="1">
+        <f t="array" ref="M8">_xll.SDK.Factors.Kh_Tension(C8,A8,B8)</f>
+        <v>1.0717734625362931</v>
+      </c>
+      <c r="N8" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L8,C8,E8,F8,M8,1,0),2)</f>
+        <v>0.11</v>
+      </c>
+      <c r="O8" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>100</v>
       </c>
@@ -750,8 +959,28 @@
         <v>45084</v>
       </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="4" t="str" cm="1">
+        <f t="array" ref="K9">_xll.SDK.Utilities.CreateRectangularCrossSection(A9,B9,C9)</f>
+        <v>CS_R_100x200_C24</v>
+      </c>
+      <c r="L9" s="8" cm="1">
+        <f t="array" ref="L9">_xll.SDK.CrossSection_StressCompute.NormalForce(D9,K9)</f>
+        <v>5</v>
+      </c>
+      <c r="M9" s="8" cm="1">
+        <f t="array" ref="M9">_xll.SDK.Factors.Kh_Tension(C9,A9,B9)</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L9,C9,E9,F9,M9,1,0),2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O9" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>100</v>
       </c>
@@ -779,8 +1008,28 @@
       <c r="I10" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="4" t="str" cm="1">
+        <f t="array" ref="K10">_xll.SDK.Utilities.CreateRectangularCrossSection(A10,B10,C10)</f>
+        <v>CS_R_100x100_C24</v>
+      </c>
+      <c r="L10" s="8" cm="1">
+        <f t="array" ref="L10">_xll.SDK.CrossSection_StressCompute.NormalForce(D10,K10)</f>
+        <v>10</v>
+      </c>
+      <c r="M10" s="8" cm="1">
+        <f t="array" ref="M10">_xll.SDK.Factors.Kh_Tension(C10,A10,B10)</f>
+        <v>1.0844717711976986</v>
+      </c>
+      <c r="N10" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L10,C10,E10,F10,M10,1,0),2)</f>
+        <v>1.38</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>200</v>
       </c>
@@ -808,8 +1057,28 @@
       <c r="I11" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="4" t="str" cm="1">
+        <f t="array" ref="K11">_xll.SDK.Utilities.CreateRectangularCrossSection(A11,B11,C11)</f>
+        <v>CS_R_200x600_C24</v>
+      </c>
+      <c r="L11" s="8" cm="1">
+        <f t="array" ref="L11">_xll.SDK.CrossSection_StressCompute.NormalForce(D11,K11)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M11" s="8" cm="1">
+        <f t="array" ref="M11">_xll.SDK.Factors.Kh_Tension(C11,A11,B11)</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L11,C11,E11,F11,M11,1,0),2)</f>
+        <v>0.12</v>
+      </c>
+      <c r="O11" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>80</v>
       </c>
@@ -837,8 +1106,28 @@
       <c r="I12" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="4" t="str" cm="1">
+        <f t="array" ref="K12">_xll.SDK.Utilities.CreateRectangularCrossSection(A12,B12,C12)</f>
+        <v>CS_R_80x120_D30</v>
+      </c>
+      <c r="L12" s="8" cm="1">
+        <f t="array" ref="L12">_xll.SDK.CrossSection_StressCompute.NormalForce(D12,K12)</f>
+        <v>10.416666666666666</v>
+      </c>
+      <c r="M12" s="8" cm="1">
+        <f t="array" ref="M12">_xll.SDK.Factors.Kh_Tension(C12,A12,B12)</f>
+        <v>1.0456395525912732</v>
+      </c>
+      <c r="N12" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L12,C12,E12,F12,M12,1,0),2)</f>
+        <v>0.9</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>100</v>
       </c>
@@ -866,8 +1155,28 @@
       <c r="I13" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="4" t="str" cm="1">
+        <f t="array" ref="K13">_xll.SDK.Utilities.CreateRectangularCrossSection(A13,B13,C13)</f>
+        <v>CS_R_100x160_D30</v>
+      </c>
+      <c r="L13" s="8" cm="1">
+        <f t="array" ref="L13">_xll.SDK.CrossSection_StressCompute.NormalForce(D13,K13)</f>
+        <v>6.25</v>
+      </c>
+      <c r="M13" s="8" cm="1">
+        <f t="array" ref="M13">_xll.SDK.Factors.Kh_Tension(C13,A13,B13)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L13,C13,E13,F13,M13,1,0),2)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O13" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>200</v>
       </c>
@@ -895,10 +1204,31 @@
       <c r="I14" s="5">
         <v>45084</v>
       </c>
+      <c r="K14" s="4" t="str" cm="1">
+        <f t="array" ref="K14">_xll.SDK.Utilities.CreateRectangularCrossSection(A14,B14,C14)</f>
+        <v>CS_R_200x300_D30</v>
+      </c>
+      <c r="L14" s="8" cm="1">
+        <f t="array" ref="L14">_xll.SDK.CrossSection_StressCompute.NormalForce(D14,K14)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M14" s="8" cm="1">
+        <f t="array" ref="M14">_xll.SDK.Factors.Kh_Tension(C14,A14,B14)</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L14,C14,E14,F14,M14,1,0),2)</f>
+        <v>0.15</v>
+      </c>
+      <c r="O14" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="K1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1321,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA7B66F-B39C-42A9-9737-F6B268D3A799}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
error with ExcelDNA integration
</commit_message>
<xml_diff>
--- a/StructuraldesignKitTesting/TestData/Test_CrossSections.xlsx
+++ b/StructuraldesignKitTesting/TestData/Test_CrossSections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume Caussarieu\source\repos\StructuralDesignKit_Holz\StructuraldesignKitTesting\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc\source\repos\StructuralDesignKit\StructuraldesignKitTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B05F0D-C5A7-4326-B5B8-F20B77B0E452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1731B3C1-22FD-4E69-AC4F-A8B4749F166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{971BC0E7-8629-419A-B2CB-730A67335DFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{971BC0E7-8629-419A-B2CB-730A67335DFF}"/>
   </bookViews>
   <sheets>
     <sheet name="TensionParallelToGrain" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="30">
   <si>
     <t>B</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>SDK Excel implementation</t>
+  </si>
+  <si>
+    <t>Stress My</t>
+  </si>
+  <si>
+    <t>Stress Mz</t>
+  </si>
+  <si>
+    <t>khy</t>
+  </si>
+  <si>
+    <t>khz</t>
   </si>
 </sst>
 </file>
@@ -214,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,14 +239,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -555,39 +564,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D737A44-6696-40E2-A70F-6CB1F0298E3A}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="8.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -615,23 +624,23 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>100</v>
       </c>
@@ -663,24 +672,24 @@
         <f t="array" ref="K3">_xll.SDK.Utilities.CreateRectangularCrossSection(A3,B3,C3)</f>
         <v>CS_R_100x200_GL24h</v>
       </c>
-      <c r="L3" s="8" cm="1">
+      <c r="L3" s="6" cm="1">
         <f t="array" ref="L3">_xll.SDK.CrossSection_StressCompute.NormalForce(D3,K3)</f>
         <v>5</v>
       </c>
-      <c r="M3" s="8" cm="1">
+      <c r="M3" s="6" cm="1">
         <f t="array" ref="M3">_xll.SDK.Factors.Kh_Tension(C3,A3,B3)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L3,C3,E3,F3,M3,1,0),2)</f>
         <v>0.51</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <f>N3/G3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>100</v>
       </c>
@@ -713,24 +722,24 @@
         <f t="array" ref="K4">_xll.SDK.Utilities.CreateRectangularCrossSection(A4,B4,C4)</f>
         <v>CS_R_100x100_GL24h</v>
       </c>
-      <c r="L4" s="8" cm="1">
+      <c r="L4" s="6" cm="1">
         <f t="array" ref="L4">_xll.SDK.CrossSection_StressCompute.NormalForce(D4,K4)</f>
         <v>10</v>
       </c>
-      <c r="M4" s="8" cm="1">
+      <c r="M4" s="6" cm="1">
         <f t="array" ref="M4">_xll.SDK.Factors.Kh_Tension(C4,A4,B4)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L4,C4,E4,F4,M4,1,0),2)</f>
         <v>1.03</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <f t="shared" ref="O4:O14" si="0">N4/G4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>200</v>
       </c>
@@ -763,24 +772,24 @@
         <f t="array" ref="K5">_xll.SDK.Utilities.CreateRectangularCrossSection(A5,B5,C5)</f>
         <v>CS_R_200x600_GL24h</v>
       </c>
-      <c r="L5" s="8" cm="1">
+      <c r="L5" s="6" cm="1">
         <f t="array" ref="L5">_xll.SDK.CrossSection_StressCompute.NormalForce(D5,K5)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M5" s="8" cm="1">
+      <c r="M5" s="6" cm="1">
         <f t="array" ref="M5">_xll.SDK.Factors.Kh_Tension(C5,A5,B5)</f>
         <v>1</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L5,C5,E5,F5,M5,1,0),2)</f>
         <v>0.09</v>
       </c>
-      <c r="O5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>80</v>
       </c>
@@ -813,24 +822,24 @@
         <f t="array" ref="K6">_xll.SDK.Utilities.CreateRectangularCrossSection(A6,B6,C6)</f>
         <v>CS_R_80x120_GL28h</v>
       </c>
-      <c r="L6" s="8" cm="1">
+      <c r="L6" s="6" cm="1">
         <f t="array" ref="L6">_xll.SDK.CrossSection_StressCompute.NormalForce(D6,K6)</f>
         <v>10.416666666666666</v>
       </c>
-      <c r="M6" s="8" cm="1">
+      <c r="M6" s="6" cm="1">
         <f t="array" ref="M6">_xll.SDK.Factors.Kh_Tension(C6,A6,B6)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L6,C6,E6,F6,M6,1,0),2)</f>
         <v>0.69</v>
       </c>
-      <c r="O6" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>100</v>
       </c>
@@ -863,24 +872,24 @@
         <f t="array" ref="K7">_xll.SDK.Utilities.CreateRectangularCrossSection(A7,B7,C7)</f>
         <v>CS_R_100x160_GL28h</v>
       </c>
-      <c r="L7" s="8" cm="1">
+      <c r="L7" s="6" cm="1">
         <f t="array" ref="L7">_xll.SDK.CrossSection_StressCompute.NormalForce(D7,K7)</f>
         <v>6.25</v>
       </c>
-      <c r="M7" s="8" cm="1">
+      <c r="M7" s="6" cm="1">
         <f t="array" ref="M7">_xll.SDK.Factors.Kh_Tension(C7,A7,B7)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L7,C7,E7,F7,M7,1,0),2)</f>
         <v>0.41</v>
       </c>
-      <c r="O7" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>200</v>
       </c>
@@ -913,24 +922,24 @@
         <f t="array" ref="K8">_xll.SDK.Utilities.CreateRectangularCrossSection(A8,B8,C8)</f>
         <v>CS_R_200x300_GL28h</v>
       </c>
-      <c r="L8" s="8" cm="1">
+      <c r="L8" s="6" cm="1">
         <f t="array" ref="L8">_xll.SDK.CrossSection_StressCompute.NormalForce(D8,K8)</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="M8" s="8" cm="1">
+      <c r="M8" s="6" cm="1">
         <f t="array" ref="M8">_xll.SDK.Factors.Kh_Tension(C8,A8,B8)</f>
         <v>1.0717734625362931</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L8,C8,E8,F8,M8,1,0),2)</f>
         <v>0.11</v>
       </c>
-      <c r="O8" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>100</v>
       </c>
@@ -963,24 +972,24 @@
         <f t="array" ref="K9">_xll.SDK.Utilities.CreateRectangularCrossSection(A9,B9,C9)</f>
         <v>CS_R_100x200_C24</v>
       </c>
-      <c r="L9" s="8" cm="1">
+      <c r="L9" s="6" cm="1">
         <f t="array" ref="L9">_xll.SDK.CrossSection_StressCompute.NormalForce(D9,K9)</f>
         <v>5</v>
       </c>
-      <c r="M9" s="8" cm="1">
+      <c r="M9" s="6" cm="1">
         <f t="array" ref="M9">_xll.SDK.Factors.Kh_Tension(C9,A9,B9)</f>
         <v>1</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L9,C9,E9,F9,M9,1,0),2)</f>
         <v>0.75</v>
       </c>
-      <c r="O9" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>100</v>
       </c>
@@ -1012,24 +1021,24 @@
         <f t="array" ref="K10">_xll.SDK.Utilities.CreateRectangularCrossSection(A10,B10,C10)</f>
         <v>CS_R_100x100_C24</v>
       </c>
-      <c r="L10" s="8" cm="1">
+      <c r="L10" s="6" cm="1">
         <f t="array" ref="L10">_xll.SDK.CrossSection_StressCompute.NormalForce(D10,K10)</f>
         <v>10</v>
       </c>
-      <c r="M10" s="8" cm="1">
+      <c r="M10" s="6" cm="1">
         <f t="array" ref="M10">_xll.SDK.Factors.Kh_Tension(C10,A10,B10)</f>
         <v>1.0844717711976986</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L10,C10,E10,F10,M10,1,0),2)</f>
         <v>1.38</v>
       </c>
-      <c r="O10" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>200</v>
       </c>
@@ -1061,24 +1070,24 @@
         <f t="array" ref="K11">_xll.SDK.Utilities.CreateRectangularCrossSection(A11,B11,C11)</f>
         <v>CS_R_200x600_C24</v>
       </c>
-      <c r="L11" s="8" cm="1">
+      <c r="L11" s="6" cm="1">
         <f t="array" ref="L11">_xll.SDK.CrossSection_StressCompute.NormalForce(D11,K11)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M11" s="8" cm="1">
+      <c r="M11" s="6" cm="1">
         <f t="array" ref="M11">_xll.SDK.Factors.Kh_Tension(C11,A11,B11)</f>
         <v>1</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L11,C11,E11,F11,M11,1,0),2)</f>
         <v>0.12</v>
       </c>
-      <c r="O11" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O11" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>80</v>
       </c>
@@ -1110,24 +1119,24 @@
         <f t="array" ref="K12">_xll.SDK.Utilities.CreateRectangularCrossSection(A12,B12,C12)</f>
         <v>CS_R_80x120_D30</v>
       </c>
-      <c r="L12" s="8" cm="1">
+      <c r="L12" s="6" cm="1">
         <f t="array" ref="L12">_xll.SDK.CrossSection_StressCompute.NormalForce(D12,K12)</f>
         <v>10.416666666666666</v>
       </c>
-      <c r="M12" s="8" cm="1">
+      <c r="M12" s="6" cm="1">
         <f t="array" ref="M12">_xll.SDK.Factors.Kh_Tension(C12,A12,B12)</f>
         <v>1.0456395525912732</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L12,C12,E12,F12,M12,1,0),2)</f>
         <v>0.9</v>
       </c>
-      <c r="O12" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>100</v>
       </c>
@@ -1159,24 +1168,24 @@
         <f t="array" ref="K13">_xll.SDK.Utilities.CreateRectangularCrossSection(A13,B13,C13)</f>
         <v>CS_R_100x160_D30</v>
       </c>
-      <c r="L13" s="8" cm="1">
+      <c r="L13" s="6" cm="1">
         <f t="array" ref="L13">_xll.SDK.CrossSection_StressCompute.NormalForce(D13,K13)</f>
         <v>6.25</v>
       </c>
-      <c r="M13" s="8" cm="1">
+      <c r="M13" s="6" cm="1">
         <f t="array" ref="M13">_xll.SDK.Factors.Kh_Tension(C13,A13,B13)</f>
         <v>1</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L13,C13,E13,F13,M13,1,0),2)</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="O13" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>200</v>
       </c>
@@ -1208,19 +1217,19 @@
         <f t="array" ref="K14">_xll.SDK.Utilities.CreateRectangularCrossSection(A14,B14,C14)</f>
         <v>CS_R_200x300_D30</v>
       </c>
-      <c r="L14" s="8" cm="1">
+      <c r="L14" s="6" cm="1">
         <f t="array" ref="L14">_xll.SDK.CrossSection_StressCompute.NormalForce(D14,K14)</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="M14" s="8" cm="1">
+      <c r="M14" s="6" cm="1">
         <f t="array" ref="M14">_xll.SDK.Factors.Kh_Tension(C14,A14,B14)</f>
         <v>1</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="6">
         <f>ROUND(_xll.SDK.CrossSectionChecks.TensionParallelToGrain_6.1.2(L14,C14,E14,F14,M14,1,0),2)</f>
         <v>0.15</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1237,32 +1246,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023A9510-5D9A-4E42-9E75-8B59D1B40438}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K1" sqref="K1:O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="1" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="K1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1290,8 +1307,23 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>100</v>
       </c>
@@ -1319,8 +1351,28 @@
       <c r="I3" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" s="4" t="str" cm="1">
+        <f t="array" ref="K3">_xll.SDK.Utilities.CreateRectangularCrossSection(A3,B3,C3)</f>
+        <v>CS_R_100x200_GL24h</v>
+      </c>
+      <c r="L3" s="6" cm="1">
+        <f t="array" ref="L3">_xll.SDK.CrossSection_StressCompute.NormalForce(D3,K3)</f>
+        <v>5</v>
+      </c>
+      <c r="M3" s="6" cm="1">
+        <f t="array" ref="M3">_xll.SDK.Factors.Kh_Tension(C3,B3)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N3" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L3,C3,E3,F3,0),2)</f>
+        <v>0.45</v>
+      </c>
+      <c r="O3" s="7">
+        <f>N3/G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>100</v>
       </c>
@@ -1348,8 +1400,28 @@
       <c r="I4" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" s="4" t="str" cm="1">
+        <f t="array" ref="K4">_xll.SDK.Utilities.CreateRectangularCrossSection(A4,B4,C4)</f>
+        <v>CS_R_100x100_GL24h</v>
+      </c>
+      <c r="L4" s="6" cm="1">
+        <f t="array" ref="L4">_xll.SDK.CrossSection_StressCompute.NormalForce(D4,K4)</f>
+        <v>10</v>
+      </c>
+      <c r="M4" s="6" cm="1">
+        <f t="array" ref="M4">_xll.SDK.Factors.Kh_Tension(C4,B4)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N4" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L4,C4,E4,F4,0),2)</f>
+        <v>0.9</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" ref="O4:O14" si="0">N4/G4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>200</v>
       </c>
@@ -1377,8 +1449,28 @@
       <c r="I5" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5" s="4" t="str" cm="1">
+        <f t="array" ref="K5">_xll.SDK.Utilities.CreateRectangularCrossSection(A5,B5,C5)</f>
+        <v>CS_R_200x600_GL24h</v>
+      </c>
+      <c r="L5" s="6" cm="1">
+        <f t="array" ref="L5">_xll.SDK.CrossSection_StressCompute.NormalForce(D5,K5)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M5" s="6" cm="1">
+        <f t="array" ref="M5">_xll.SDK.Factors.Kh_Tension(C5,B5)</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L5,C5,E5,F5,0),2)</f>
+        <v>0.08</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>80</v>
       </c>
@@ -1406,8 +1498,28 @@
       <c r="I6" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6" s="4" t="str" cm="1">
+        <f t="array" ref="K6">_xll.SDK.Utilities.CreateRectangularCrossSection(A6,B6,C6)</f>
+        <v>CS_R_80x120_GL28h</v>
+      </c>
+      <c r="L6" s="6" cm="1">
+        <f t="array" ref="L6">_xll.SDK.CrossSection_StressCompute.NormalForce(D6,K6)</f>
+        <v>10.416666666666666</v>
+      </c>
+      <c r="M6" s="6" cm="1">
+        <f t="array" ref="M6">_xll.SDK.Factors.Kh_Tension(C6,B6)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N6" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L6,C6,E6,F6,0),2)</f>
+        <v>0.6</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>100</v>
       </c>
@@ -1435,8 +1547,28 @@
       <c r="I7" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="str" cm="1">
+        <f t="array" ref="K7">_xll.SDK.Utilities.CreateRectangularCrossSection(A7,B7,C7)</f>
+        <v>CS_R_100x160_GL28h</v>
+      </c>
+      <c r="L7" s="6" cm="1">
+        <f t="array" ref="L7">_xll.SDK.CrossSection_StressCompute.NormalForce(D7,K7)</f>
+        <v>6.25</v>
+      </c>
+      <c r="M7" s="6" cm="1">
+        <f t="array" ref="M7">_xll.SDK.Factors.Kh_Tension(C7,B7)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N7" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L7,C7,E7,F7,0),2)</f>
+        <v>0.36</v>
+      </c>
+      <c r="O7" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>200</v>
       </c>
@@ -1464,8 +1596,28 @@
       <c r="I8" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K8" s="4" t="str" cm="1">
+        <f t="array" ref="K8">_xll.SDK.Utilities.CreateRectangularCrossSection(A8,B8,C8)</f>
+        <v>CS_R_200x300_GL28h</v>
+      </c>
+      <c r="L8" s="6" cm="1">
+        <f t="array" ref="L8">_xll.SDK.CrossSection_StressCompute.NormalForce(D8,K8)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M8" s="6" cm="1">
+        <f t="array" ref="M8">_xll.SDK.Factors.Kh_Tension(C8,B8)</f>
+        <v>1.0717734625362931</v>
+      </c>
+      <c r="N8" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L8,C8,E8,F8,0),2)</f>
+        <v>0.1</v>
+      </c>
+      <c r="O8" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>100</v>
       </c>
@@ -1493,8 +1645,28 @@
       <c r="I9" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K9" s="4" t="str" cm="1">
+        <f t="array" ref="K9">_xll.SDK.Utilities.CreateRectangularCrossSection(A9,B9,C9)</f>
+        <v>CS_R_100x200_C24</v>
+      </c>
+      <c r="L9" s="6" cm="1">
+        <f t="array" ref="L9">_xll.SDK.CrossSection_StressCompute.NormalForce(D9,K9)</f>
+        <v>5</v>
+      </c>
+      <c r="M9" s="6" cm="1">
+        <f t="array" ref="M9">_xll.SDK.Factors.Kh_Tension(C9,B9)</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L9,C9,E9,F9,0),2)</f>
+        <v>0.52</v>
+      </c>
+      <c r="O9" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>100</v>
       </c>
@@ -1522,8 +1694,28 @@
       <c r="I10" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K10" s="4" t="str" cm="1">
+        <f t="array" ref="K10">_xll.SDK.Utilities.CreateRectangularCrossSection(A10,B10,C10)</f>
+        <v>CS_R_100x100_C24</v>
+      </c>
+      <c r="L10" s="6" cm="1">
+        <f t="array" ref="L10">_xll.SDK.CrossSection_StressCompute.NormalForce(D10,K10)</f>
+        <v>10</v>
+      </c>
+      <c r="M10" s="6" cm="1">
+        <f t="array" ref="M10">_xll.SDK.Factors.Kh_Tension(C10,B10)</f>
+        <v>1.0844717711976986</v>
+      </c>
+      <c r="N10" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L10,C10,E10,F10,0),2)</f>
+        <v>1.03</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>200</v>
       </c>
@@ -1551,8 +1743,28 @@
       <c r="I11" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K11" s="4" t="str" cm="1">
+        <f t="array" ref="K11">_xll.SDK.Utilities.CreateRectangularCrossSection(A11,B11,C11)</f>
+        <v>CS_R_200x600_C24</v>
+      </c>
+      <c r="L11" s="6" cm="1">
+        <f t="array" ref="L11">_xll.SDK.CrossSection_StressCompute.NormalForce(D11,K11)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M11" s="6" cm="1">
+        <f t="array" ref="M11">_xll.SDK.Factors.Kh_Tension(C11,B11)</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L11,C11,E11,F11,0),2)</f>
+        <v>0.09</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>80</v>
       </c>
@@ -1580,8 +1792,28 @@
       <c r="I12" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K12" s="4" t="str" cm="1">
+        <f t="array" ref="K12">_xll.SDK.Utilities.CreateRectangularCrossSection(A12,B12,C12)</f>
+        <v>CS_R_80x120_D30</v>
+      </c>
+      <c r="L12" s="6" cm="1">
+        <f t="array" ref="L12">_xll.SDK.CrossSection_StressCompute.NormalForce(D12,K12)</f>
+        <v>10.416666666666666</v>
+      </c>
+      <c r="M12" s="6" cm="1">
+        <f t="array" ref="M12">_xll.SDK.Factors.Kh_Tension(C12,B12)</f>
+        <v>1.0456395525912732</v>
+      </c>
+      <c r="N12" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L12,C12,E12,F12,0),2)</f>
+        <v>0.71</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>100</v>
       </c>
@@ -1609,8 +1841,28 @@
       <c r="I13" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K13" s="4" t="str" cm="1">
+        <f t="array" ref="K13">_xll.SDK.Utilities.CreateRectangularCrossSection(A13,B13,C13)</f>
+        <v>CS_R_100x160_D30</v>
+      </c>
+      <c r="L13" s="6" cm="1">
+        <f t="array" ref="L13">_xll.SDK.CrossSection_StressCompute.NormalForce(D13,K13)</f>
+        <v>6.25</v>
+      </c>
+      <c r="M13" s="6" cm="1">
+        <f t="array" ref="M13">_xll.SDK.Factors.Kh_Tension(C13,B13)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L13,C13,E13,F13,0),2)</f>
+        <v>0.42</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>200</v>
       </c>
@@ -1638,10 +1890,31 @@
       <c r="I14" s="5">
         <v>45084</v>
       </c>
+      <c r="K14" s="4" t="str" cm="1">
+        <f t="array" ref="K14">_xll.SDK.Utilities.CreateRectangularCrossSection(A14,B14,C14)</f>
+        <v>CS_R_200x300_D30</v>
+      </c>
+      <c r="L14" s="6" cm="1">
+        <f t="array" ref="L14">_xll.SDK.CrossSection_StressCompute.NormalForce(D14,K14)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="M14" s="6" cm="1">
+        <f t="array" ref="M14">_xll.SDK.Factors.Kh_Tension(C14,B14)</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.CompressionParallelToGrain_6.1.4(L14,C14,E14,F14,0),2)</f>
+        <v>0.11</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="K1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1649,33 +1922,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA7B66F-B39C-42A9-9737-F6B268D3A799}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="18" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="L1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1706,8 +1991,29 @@
       <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>100</v>
       </c>
@@ -1738,8 +2044,36 @@
       <c r="J3" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="4" t="str" cm="1">
+        <f t="array" ref="L3">_xll.SDK.Utilities.CreateRectangularCrossSection(A3,B3,C3)</f>
+        <v>CS_R_100x160_D30</v>
+      </c>
+      <c r="M3" s="6" cm="1">
+        <f t="array" ref="M3">_xll.SDK.CrossSection_StressCompute.BendingY(D3,$L3)</f>
+        <v>11.71875</v>
+      </c>
+      <c r="N3" s="6" cm="1">
+        <f t="array" ref="N3">_xll.SDK.CrossSection_StressCompute.BendingZ(E3,$L3)</f>
+        <v>7.4999999999999991</v>
+      </c>
+      <c r="O3" s="6" cm="1">
+        <f t="array" ref="O3">_xll.SDK.Factors.Kh_Bending(C3,B3)</f>
+        <v>1</v>
+      </c>
+      <c r="P3" s="6" cm="1">
+        <f t="array" ref="P3">_xll.SDK.Factors.Kh_Bending(C3,A3)</f>
+        <v>1.0844717711976986</v>
+      </c>
+      <c r="Q3" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M3,N3,L3,F3,G3,O3,P3,0),2)</f>
+        <v>0.9</v>
+      </c>
+      <c r="R3" s="7">
+        <f>Q3/H3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>100</v>
       </c>
@@ -1770,8 +2104,35 @@
       <c r="J4" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="4" t="str" cm="1">
+        <f t="array" ref="L4">_xll.SDK.Utilities.CreateRectangularCrossSection(A4,B4,C4)</f>
+        <v>CS_R_100x200_GL24h</v>
+      </c>
+      <c r="M4" s="6" cm="1">
+        <f t="array" ref="M4">_xll.SDK.CrossSection_StressCompute.BendingY(D4,$L4)</f>
+        <v>7.5</v>
+      </c>
+      <c r="N4" s="6" cm="1">
+        <f t="array" ref="N4">_xll.SDK.CrossSection_StressCompute.BendingZ(E4,$L4)</f>
+        <v>6</v>
+      </c>
+      <c r="O4" s="6" cm="1">
+        <f t="array" ref="O4">_xll.SDK.Factors.Kh_Bending(C4,B4)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M4,N4,L4,F4,G4,O4,P4,0),2)</f>
+        <v>0.99</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" ref="R4:R14" si="0">Q4/H4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>100</v>
       </c>
@@ -1802,8 +2163,35 @@
       <c r="J5" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L5" s="4" t="str" cm="1">
+        <f t="array" ref="L5">_xll.SDK.Utilities.CreateRectangularCrossSection(A5,B5,C5)</f>
+        <v>CS_R_100x100_GL24h</v>
+      </c>
+      <c r="M5" s="6" cm="1">
+        <f t="array" ref="M5">_xll.SDK.CrossSection_StressCompute.BendingY(D5,$L5)</f>
+        <v>30</v>
+      </c>
+      <c r="N5" s="6" cm="1">
+        <f t="array" ref="N5">_xll.SDK.CrossSection_StressCompute.BendingZ(E5,$L5)</f>
+        <v>12</v>
+      </c>
+      <c r="O5" s="6" cm="1">
+        <f t="array" ref="O5">_xll.SDK.Factors.Kh_Bending(C5,B5)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M5,N5,L5,F5,G5,O5,P5,0),2)</f>
+        <v>3.22</v>
+      </c>
+      <c r="R5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>200</v>
       </c>
@@ -1834,8 +2222,35 @@
       <c r="J6" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="4" t="str" cm="1">
+        <f t="array" ref="L6">_xll.SDK.Utilities.CreateRectangularCrossSection(A6,B6,C6)</f>
+        <v>CS_R_200x700_GL24h</v>
+      </c>
+      <c r="M6" s="6" cm="1">
+        <f t="array" ref="M6">_xll.SDK.CrossSection_StressCompute.BendingY(D6,$L6)</f>
+        <v>0.30612244897959184</v>
+      </c>
+      <c r="N6" s="6" cm="1">
+        <f t="array" ref="N6">_xll.SDK.CrossSection_StressCompute.BendingZ(E6,$L6)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="O6" s="6" cm="1">
+        <f t="array" ref="O6">_xll.SDK.Factors.Kh_Bending(C6,B6)</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M6,N6,L6,F6,G6,O6,P6,0),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>80</v>
       </c>
@@ -1866,8 +2281,35 @@
       <c r="J7" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="4" t="str" cm="1">
+        <f t="array" ref="L7">_xll.SDK.Utilities.CreateRectangularCrossSection(A7,B7,C7)</f>
+        <v>CS_R_80x120_GL28h</v>
+      </c>
+      <c r="M7" s="6" cm="1">
+        <f t="array" ref="M7">_xll.SDK.CrossSection_StressCompute.BendingY(D7,$L7)</f>
+        <v>26.041666666666668</v>
+      </c>
+      <c r="N7" s="6" cm="1">
+        <f t="array" ref="N7">_xll.SDK.CrossSection_StressCompute.BendingZ(E7,$L7)</f>
+        <v>15.625</v>
+      </c>
+      <c r="O7" s="6" cm="1">
+        <f t="array" ref="O7">_xll.SDK.Factors.Kh_Bending(C7,B7)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M7,N7,L7,F7,G7,O7,P7,0),2)</f>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>100</v>
       </c>
@@ -1898,8 +2340,35 @@
       <c r="J8" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L8" s="4" t="str" cm="1">
+        <f t="array" ref="L8">_xll.SDK.Utilities.CreateRectangularCrossSection(A8,B8,C8)</f>
+        <v>CS_R_100x160_GL28h</v>
+      </c>
+      <c r="M8" s="6" cm="1">
+        <f t="array" ref="M8">_xll.SDK.CrossSection_StressCompute.BendingY(D8,$L8)</f>
+        <v>11.71875</v>
+      </c>
+      <c r="N8" s="6" cm="1">
+        <f t="array" ref="N8">_xll.SDK.CrossSection_StressCompute.BendingZ(E8,$L8)</f>
+        <v>7.4999999999999991</v>
+      </c>
+      <c r="O8" s="6" cm="1">
+        <f t="array" ref="O8">_xll.SDK.Factors.Kh_Bending(C8,B8)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M8,N8,L8,F8,G8,O8,P8,0),2)</f>
+        <v>0.92</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>200</v>
       </c>
@@ -1930,8 +2399,36 @@
       <c r="J9" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="4" t="str" cm="1">
+        <f t="array" ref="L9">_xll.SDK.Utilities.CreateRectangularCrossSection(A9,B9,C9)</f>
+        <v>CS_R_200x300_GL28h</v>
+      </c>
+      <c r="M9" s="6" cm="1">
+        <f t="array" ref="M9">_xll.SDK.CrossSection_StressCompute.BendingY(D9,$L9)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="N9" s="6" cm="1">
+        <f t="array" ref="N9">_xll.SDK.CrossSection_StressCompute.BendingZ(E9,$L9)</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="6" cm="1">
+        <f t="array" ref="O9">_xll.SDK.Factors.Kh_Bending(C9,B9)</f>
+        <v>1.0717734625362931</v>
+      </c>
+      <c r="P9" s="6" cm="1">
+        <f t="array" ref="P9">_xll.SDK.Factors.Kh_Bending(C9,A9)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M9,N9,L9,F9,G9,O9,P9,0),2)</f>
+        <v>0.13</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>300</v>
       </c>
@@ -1962,8 +2459,35 @@
       <c r="J10" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="4" t="str" cm="1">
+        <f t="array" ref="L10">_xll.SDK.Utilities.CreateRectangularCrossSection(A10,B10,C10)</f>
+        <v>CS_R_300x300_GL24h</v>
+      </c>
+      <c r="M10" s="6" cm="1">
+        <f t="array" ref="M10">_xll.SDK.CrossSection_StressCompute.BendingY(D10,$L10)</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="N10" s="6" cm="1">
+        <f t="array" ref="N10">_xll.SDK.CrossSection_StressCompute.BendingZ(E10,$L10)</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="O10" s="6" cm="1">
+        <f t="array" ref="O10">_xll.SDK.Factors.Kh_Bending(C10,B10)</f>
+        <v>1.0717734625362931</v>
+      </c>
+      <c r="P10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M10,N10,L10,F10,G10,O10,P10,0),2)</f>
+        <v>0.26</v>
+      </c>
+      <c r="R10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0116731517509727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>100</v>
       </c>
@@ -1994,8 +2518,36 @@
       <c r="J11" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="4" t="str" cm="1">
+        <f t="array" ref="L11">_xll.SDK.Utilities.CreateRectangularCrossSection(A11,B11,C11)</f>
+        <v>CS_R_100x200_C24</v>
+      </c>
+      <c r="M11" s="6" cm="1">
+        <f t="array" ref="M11">_xll.SDK.CrossSection_StressCompute.BendingY(D11,$L11)</f>
+        <v>7.5</v>
+      </c>
+      <c r="N11" s="6" cm="1">
+        <f t="array" ref="N11">_xll.SDK.CrossSection_StressCompute.BendingZ(E11,$L11)</f>
+        <v>6</v>
+      </c>
+      <c r="O11" s="6" cm="1">
+        <f t="array" ref="O11">_xll.SDK.Factors.Kh_Bending(C11,B11)</f>
+        <v>1</v>
+      </c>
+      <c r="P11" s="6" cm="1">
+        <f t="array" ref="P11">_xll.SDK.Factors.Kh_Bending(C11,A11)</f>
+        <v>1.0844717711976986</v>
+      </c>
+      <c r="Q11" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M11,N11,L11,F11,G11,O11,P11,0),2)</f>
+        <v>1.03</v>
+      </c>
+      <c r="R11" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>100</v>
       </c>
@@ -2026,8 +2578,36 @@
       <c r="J12" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="4" t="str" cm="1">
+        <f t="array" ref="L12">_xll.SDK.Utilities.CreateRectangularCrossSection(A12,B12,C12)</f>
+        <v>CS_R_100x100_C24</v>
+      </c>
+      <c r="M12" s="6" cm="1">
+        <f t="array" ref="M12">_xll.SDK.CrossSection_StressCompute.BendingY(D12,$L12)</f>
+        <v>30</v>
+      </c>
+      <c r="N12" s="6" cm="1">
+        <f t="array" ref="N12">_xll.SDK.CrossSection_StressCompute.BendingZ(E12,$L12)</f>
+        <v>12</v>
+      </c>
+      <c r="O12" s="6" cm="1">
+        <f t="array" ref="O12">_xll.SDK.Factors.Kh_Bending(C12,B12)</f>
+        <v>1.0844717711976986</v>
+      </c>
+      <c r="P12" s="6" cm="1">
+        <f t="array" ref="P12">_xll.SDK.Factors.Kh_Bending(C12,A12)</f>
+        <v>1.0844717711976986</v>
+      </c>
+      <c r="Q12" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M12,N12,L12,F12,G12,O12,P12,0),2)</f>
+        <v>3.2</v>
+      </c>
+      <c r="R12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>200</v>
       </c>
@@ -2058,8 +2638,36 @@
       <c r="J13" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="4" t="str" cm="1">
+        <f t="array" ref="L13">_xll.SDK.Utilities.CreateRectangularCrossSection(A13,B13,C13)</f>
+        <v>CS_R_200x600_C24</v>
+      </c>
+      <c r="M13" s="6" cm="1">
+        <f t="array" ref="M13">_xll.SDK.CrossSection_StressCompute.BendingY(D13,$L13)</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N13" s="6" cm="1">
+        <f t="array" ref="N13">_xll.SDK.CrossSection_StressCompute.BendingZ(E13,$L13)</f>
+        <v>0.5</v>
+      </c>
+      <c r="O13" s="6" cm="1">
+        <f t="array" ref="O13">_xll.SDK.Factors.Kh_Bending(C13,B13)</f>
+        <v>1</v>
+      </c>
+      <c r="P13" s="6" cm="1">
+        <f t="array" ref="P13">_xll.SDK.Factors.Kh_Bending(C13,A13)</f>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M13,N13,L13,F13,G13,O13,P13,0),2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R13" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>80</v>
       </c>
@@ -2090,8 +2698,36 @@
       <c r="J14" s="5">
         <v>45084</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L14" s="4" t="str" cm="1">
+        <f t="array" ref="L14">_xll.SDK.Utilities.CreateRectangularCrossSection(A14,B14,C14)</f>
+        <v>CS_R_80x120_D30</v>
+      </c>
+      <c r="M14" s="6" cm="1">
+        <f t="array" ref="M14">_xll.SDK.CrossSection_StressCompute.BendingY(D14,$L14)</f>
+        <v>26.041666666666668</v>
+      </c>
+      <c r="N14" s="6" cm="1">
+        <f t="array" ref="N14">_xll.SDK.CrossSection_StressCompute.BendingZ(E14,$L14)</f>
+        <v>15.625</v>
+      </c>
+      <c r="O14" s="6" cm="1">
+        <f t="array" ref="O14">_xll.SDK.Factors.Kh_Bending(C14,B14)</f>
+        <v>1.0456395525912732</v>
+      </c>
+      <c r="P14" s="6" cm="1">
+        <f t="array" ref="P14">_xll.SDK.Factors.Kh_Bending(C14,A14)</f>
+        <v>1.1339665776330272</v>
+      </c>
+      <c r="Q14" s="6">
+        <f>ROUND(_xll.SDK.CrossSectionChecks.Bending_6.1.6(M14,N14,L14,F14,G14,O14,P14,0),2)</f>
+        <v>1.87</v>
+      </c>
+      <c r="R14" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>200</v>
       </c>
@@ -2123,12 +2759,13 @@
         <v>45084</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="L1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2143,7 +2780,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2157,7 +2794,7 @@
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>